<commit_message>
Modification et mise en place final des instructions de la suite de Fibonacchi et finalisation du fichier xlsx contenant les explications
</commit_message>
<xml_diff>
--- a/Suite d'instruction.xlsx
+++ b/Suite d'instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18500" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="13290" windowHeight="2780"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="130">
   <si>
     <t>Traduction</t>
   </si>
@@ -114,9 +114,6 @@
     <t>00001111</t>
   </si>
   <si>
-    <t>00010000</t>
-  </si>
-  <si>
     <t>Jump à l'instruction 4</t>
   </si>
   <si>
@@ -166,6 +163,249 @@
   </si>
   <si>
     <t>2014</t>
+  </si>
+  <si>
+    <t>011001000001010</t>
+  </si>
+  <si>
+    <t>Addition de 01 et 01 dans 01</t>
+  </si>
+  <si>
+    <t>011000101010110</t>
+  </si>
+  <si>
+    <t>Init de 0001 dans le registre 10</t>
+  </si>
+  <si>
+    <t>010000000101000</t>
+  </si>
+  <si>
+    <t>Stockage de 10 dans la RAM à la case mémoire 00000001</t>
+  </si>
+  <si>
+    <t>000000011110000</t>
+  </si>
+  <si>
+    <t>Jump à l'instruction 15</t>
+  </si>
+  <si>
+    <t>00f0</t>
+  </si>
+  <si>
+    <t>320a</t>
+  </si>
+  <si>
+    <t>010000000011011</t>
+  </si>
+  <si>
+    <t>201b</t>
+  </si>
+  <si>
+    <t>Comparaison du num demandé avec 0010 si égale jump à l'instruction 13</t>
+  </si>
+  <si>
+    <t>100000011110001</t>
+  </si>
+  <si>
+    <t>40f1</t>
+  </si>
+  <si>
+    <t>00010001</t>
+  </si>
+  <si>
+    <t>00010010</t>
+  </si>
+  <si>
+    <t>00010011</t>
+  </si>
+  <si>
+    <t>00010100</t>
+  </si>
+  <si>
+    <t>00010101</t>
+  </si>
+  <si>
+    <t>00010110</t>
+  </si>
+  <si>
+    <t>00010111</t>
+  </si>
+  <si>
+    <t>Init de 0001 dans le registrre 10</t>
+  </si>
+  <si>
+    <t>Stockage dans la RAM du registre 01(cpt) en 00000010</t>
+  </si>
+  <si>
+    <t>Stcokage dans la RAM du registre 10(n) dans 00000011</t>
+  </si>
+  <si>
+    <t>Stockage dans la RAM du registre 10(n-1) dans 00000100</t>
+  </si>
+  <si>
+    <t>Commencement du FOR</t>
+  </si>
+  <si>
+    <t>Récupération de 00000010 dans le registre 01(cpt)</t>
+  </si>
+  <si>
+    <t>Récupération de 00000011 dans le registre 10(n)</t>
+  </si>
+  <si>
+    <t>Récupération de 00000100 dans le registre 11(n-1)</t>
+  </si>
+  <si>
+    <t>Addition de 10 et 11 dans le registre 11(n à partir de maintenant)</t>
+  </si>
+  <si>
+    <t>Stockage de 10 dans la RAM à la case mémoire 00000100</t>
+  </si>
+  <si>
+    <t>Stockage de 11 dans la RAM à la case mémoire 00000011</t>
+  </si>
+  <si>
+    <t>Addition de 01 et 10 dans 01(incrémentation du compteur)</t>
+  </si>
+  <si>
+    <t>00011000</t>
+  </si>
+  <si>
+    <t>00011001</t>
+  </si>
+  <si>
+    <t>00011010</t>
+  </si>
+  <si>
+    <t>00011011</t>
+  </si>
+  <si>
+    <t>00011100</t>
+  </si>
+  <si>
+    <t>00011101</t>
+  </si>
+  <si>
+    <t>00011110</t>
+  </si>
+  <si>
+    <t>00011111</t>
+  </si>
+  <si>
+    <t>00100000</t>
+  </si>
+  <si>
+    <t>00100001</t>
+  </si>
+  <si>
+    <t>00100010</t>
+  </si>
+  <si>
+    <t>00100011</t>
+  </si>
+  <si>
+    <t>00100100</t>
+  </si>
+  <si>
+    <t>00100101</t>
+  </si>
+  <si>
+    <t>Jump à l'instruction 19 (début du for)</t>
+  </si>
+  <si>
+    <t>Comparaison du num demandé avec le cpt si égale jump à l'instruction 32 (condition d'arret)</t>
+  </si>
+  <si>
+    <t>Stockage de 10 dans la case mémoire 00000010 (on retourne le résultat)</t>
+  </si>
+  <si>
+    <t>Fin du for</t>
+  </si>
+  <si>
+    <t>Remise à 0  de la RAM</t>
+  </si>
+  <si>
+    <t>Stockage de 11 dans la RAM à la case mémoire 00000100</t>
+  </si>
+  <si>
+    <t>010000000100100</t>
+  </si>
+  <si>
+    <t>010000000111000</t>
+  </si>
+  <si>
+    <t>010000001001000</t>
+  </si>
+  <si>
+    <t>001000000100100</t>
+  </si>
+  <si>
+    <t>001000000111000</t>
+  </si>
+  <si>
+    <t>001000001001100</t>
+  </si>
+  <si>
+    <t>011001111100110</t>
+  </si>
+  <si>
+    <t>010000000111100</t>
+  </si>
+  <si>
+    <t>011000101100110</t>
+  </si>
+  <si>
+    <t>Récupération de 11111111 dans le registre 11</t>
+  </si>
+  <si>
+    <t>001111111111100</t>
+  </si>
+  <si>
+    <t>000000101000000</t>
+  </si>
+  <si>
+    <t>100001000010001</t>
+  </si>
+  <si>
+    <t>104c</t>
+  </si>
+  <si>
+    <t>33e6</t>
+  </si>
+  <si>
+    <t>203c</t>
+  </si>
+  <si>
+    <t>0140</t>
+  </si>
+  <si>
+    <t>1ffc</t>
+  </si>
+  <si>
+    <t>010000001001100</t>
+  </si>
+  <si>
+    <t>204c</t>
+  </si>
+  <si>
+    <t>Stockage de 11 dans la RAM à la case mémoire 00000010</t>
+  </si>
+  <si>
+    <t>010000000011000</t>
+  </si>
+  <si>
+    <t>010000000101100</t>
+  </si>
+  <si>
+    <t>00100110</t>
+  </si>
+  <si>
+    <t>00100111</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>202c</t>
   </si>
 </sst>
 </file>
@@ -201,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -213,6 +453,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,19 +751,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="32.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
     <col min="3" max="3" width="20.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="26.90625" customWidth="1"/>
+    <col min="4" max="4" width="67.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -551,7 +795,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -575,7 +819,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>IF(B3 = "010","STORE",IF(B3 = "011","OPERATION",IF(B3 = "101","MOVE",IF(B3 = "110","RETURN",IF(B3 = "000","JUMP",IF(B3 = "100","JUMP EQUALS",IF(B3 = "001","LOAD","ERREUR")))))))</f>
@@ -593,17 +837,17 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="str">
         <f>IF(B4 = "010","STORE",IF(B4 = "011","OPERATION",IF(B4 = "101","MOVE",IF(B4 = "110","RETURN",IF(B4 = "000","JUMP",IF(B4 = "100","JUMP EQUALS",IF(B4 = "001","LOAD","ERREUR")))))))</f>
         <v>JUMP</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -620,7 +864,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f t="shared" ref="E5:E38" si="0">IF(B5 = "010","STORE",IF(B5 = "011","OPERATION",IF(B5 = "101","MOVE",IF(B5 = "110","RETURN",IF(B5 = "000","JUMP",IF(B5 = "100","JUMP EQUALS",IF(B5 = "001","LOAD","ERREUR")))))))</f>
+        <f t="shared" ref="E5:E40" si="0">IF(B5 = "010","STORE",IF(B5 = "011","OPERATION",IF(B5 = "101","MOVE",IF(B5 = "110","RETURN",IF(B5 = "000","JUMP",IF(B5 = "100","JUMP EQUALS",IF(B5 = "001","LOAD","ERREUR")))))))</f>
         <v>RETURN</v>
       </c>
       <c r="F5">
@@ -635,17 +879,17 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OPERATION</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>OPERATION</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -656,10 +900,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -677,17 +921,17 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>JUMP</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -698,17 +942,17 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>STORE</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -722,7 +966,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -736,306 +980,677 @@
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
+        <v>OPERATION</v>
+      </c>
+      <c r="F11">
+        <v>3156</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1">
+        <v>100</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
       <c r="E12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ERREUR</v>
+        <f>IF(B11 = "010","STORE",IF(B11 = "011","OPERATION",IF(B11 = "101","MOVE",IF(B11 = "110","RETURN",IF(B11 = "000","JUMP",IF(B11 = "100","JUMP EQUALS",IF(B11 = "001","LOAD","ERREUR")))))))</f>
+        <v>OPERATION</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
+        <v>JUMP</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
+        <v>OPERATION</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
+        <v>STORE</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>RETURN</v>
+      </c>
+      <c r="F16">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>OPERATION</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F18">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F19">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F20">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+        <v>LOAD</v>
+      </c>
+      <c r="F21">
+        <v>1024</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+        <v>LOAD</v>
+      </c>
+      <c r="F22">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+        <v>LOAD</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+        <v>OPERATION</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F25">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+        <v>OPERATION</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+        <v>OPERATION</v>
+      </c>
+      <c r="F28">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F29">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+        <v>LOAD</v>
+      </c>
+      <c r="F30">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+        <v>LOAD</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+        <v>JUMP EQUALS</v>
+      </c>
+      <c r="F32">
+        <v>4211</v>
+      </c>
+      <c r="G32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+        <v>JUMP</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
       <c r="E34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F34">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="E35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+        <v>LOAD</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+        <v>STORE</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" t="s">
+        <v>123</v>
+      </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ERREUR</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:5">
+        <v>STORE</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>STORE</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>RETURN</v>
+      </c>
+      <c r="F40">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:7">
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:7">
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:7">
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:7">
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:7">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:7">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:7">
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>